<commit_message>
added the data directory and ranks file
</commit_message>
<xml_diff>
--- a/scripts/state_cd_relationship.xlsx
+++ b/scripts/state_cd_relationship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varun-urbint/Documents/Constituent-Data-Collaborative/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDFED225-5C4C-924C-A263-3CD671DE4DD2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B66397-3B1F-564C-8039-190AEAB48696}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4380" yWindow="3560" windowWidth="26440" windowHeight="15440" xr2:uid="{128CA14C-B1FD-4248-9A0F-6F67D9335ED1}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="55">
   <si>
     <t>State</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Alaska</t>
-  </si>
-  <si>
-    <t>At-large</t>
   </si>
   <si>
     <t>Arizona</t>
@@ -205,7 +202,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="00"/>
+    <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -267,11 +264,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +586,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,13 +678,13 @@
       <c r="B8" s="6">
         <v>2</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>5</v>
+      <c r="C8" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="6">
         <v>4</v>
@@ -698,7 +695,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="6">
         <v>4</v>
@@ -709,7 +706,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="6">
         <v>4</v>
@@ -720,7 +717,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="6">
         <v>4</v>
@@ -731,7 +728,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="6">
         <v>4</v>
@@ -742,7 +739,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="6">
         <v>4</v>
@@ -753,7 +750,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="6">
         <v>4</v>
@@ -764,7 +761,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="6">
         <v>4</v>
@@ -775,7 +772,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="6">
         <v>4</v>
@@ -786,7 +783,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="6">
         <v>5</v>
@@ -797,7 +794,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="6">
         <v>5</v>
@@ -808,7 +805,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="6">
         <v>5</v>
@@ -819,7 +816,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="6">
         <v>5</v>
@@ -830,7 +827,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="6">
         <v>6</v>
@@ -841,7 +838,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="6">
         <v>6</v>
@@ -852,7 +849,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="6">
         <v>6</v>
@@ -863,7 +860,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="6">
         <v>6</v>
@@ -874,7 +871,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" s="6">
         <v>6</v>
@@ -885,7 +882,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="6">
         <v>6</v>
@@ -896,7 +893,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="6">
         <v>6</v>
@@ -907,7 +904,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" s="6">
         <v>6</v>
@@ -918,7 +915,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="6">
         <v>6</v>
@@ -929,7 +926,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" s="6">
         <v>6</v>
@@ -940,7 +937,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="6">
         <v>6</v>
@@ -951,7 +948,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="6">
         <v>6</v>
@@ -962,7 +959,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" s="6">
         <v>6</v>
@@ -973,7 +970,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" s="6">
         <v>6</v>
@@ -984,7 +981,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" s="6">
         <v>6</v>
@@ -995,7 +992,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="6">
         <v>6</v>
@@ -1006,7 +1003,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="6">
         <v>6</v>
@@ -1017,7 +1014,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="6">
         <v>6</v>
@@ -1028,7 +1025,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="6">
         <v>6</v>
@@ -1050,7 +1047,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" s="6">
         <v>6</v>
@@ -1061,7 +1058,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43" s="6">
         <v>6</v>
@@ -1072,7 +1069,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" s="6">
         <v>6</v>
@@ -1083,7 +1080,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45" s="6">
         <v>6</v>
@@ -1094,7 +1091,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46" s="6">
         <v>6</v>
@@ -1105,7 +1102,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" s="6">
         <v>6</v>
@@ -1116,7 +1113,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B48" s="6">
         <v>6</v>
@@ -1127,7 +1124,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B49" s="6">
         <v>6</v>
@@ -1138,7 +1135,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B50" s="6">
         <v>6</v>
@@ -1149,7 +1146,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B51" s="6">
         <v>6</v>
@@ -1160,7 +1157,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B52" s="6">
         <v>6</v>
@@ -1171,7 +1168,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B53" s="6">
         <v>6</v>
@@ -1182,7 +1179,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54" s="6">
         <v>8</v>
@@ -1193,7 +1190,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55" s="6">
         <v>9</v>
@@ -1204,7 +1201,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" s="6">
         <v>12</v>
@@ -1215,7 +1212,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" s="6">
         <v>13</v>
@@ -1226,7 +1223,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B58" s="6">
         <v>15</v>
@@ -1237,7 +1234,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B59" s="6">
         <v>16</v>
@@ -1248,7 +1245,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60" s="6">
         <v>18</v>
@@ -1259,7 +1256,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B61" s="6">
         <v>17</v>
@@ -1270,7 +1267,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" s="6">
         <v>19</v>
@@ -1281,7 +1278,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B63" s="6">
         <v>20</v>
@@ -1292,7 +1289,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B64" s="6">
         <v>21</v>
@@ -1303,7 +1300,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B65" s="6">
         <v>22</v>
@@ -1314,7 +1311,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="6">
         <v>23</v>
@@ -1325,7 +1322,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B67" s="6">
         <v>24</v>
@@ -1336,7 +1333,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B68" s="6">
         <v>25</v>
@@ -1347,7 +1344,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B69" s="6">
         <v>26</v>
@@ -1358,7 +1355,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B70" s="6">
         <v>27</v>
@@ -1369,7 +1366,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B71" s="6">
         <v>28</v>
@@ -1380,7 +1377,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B72" s="6">
         <v>29</v>
@@ -1391,7 +1388,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B73" s="6">
         <v>31</v>
@@ -1402,7 +1399,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B74" s="6">
         <v>32</v>
@@ -1413,7 +1410,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" s="6">
         <v>33</v>
@@ -1424,7 +1421,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B76" s="6">
         <v>34</v>
@@ -1435,7 +1432,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B77" s="6">
         <v>35</v>
@@ -1446,7 +1443,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B78" s="6">
         <v>36</v>
@@ -1457,7 +1454,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B79" s="6">
         <v>37</v>
@@ -1468,7 +1465,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B80" s="6">
         <v>39</v>
@@ -1479,7 +1476,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B81" s="6">
         <v>40</v>
@@ -1490,7 +1487,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B82" s="6">
         <v>41</v>
@@ -1501,7 +1498,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B83" s="6">
         <v>42</v>
@@ -1512,7 +1509,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B84" s="6">
         <v>44</v>
@@ -1523,7 +1520,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B85" s="6">
         <v>45</v>
@@ -1534,7 +1531,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B86" s="6">
         <v>47</v>
@@ -1545,7 +1542,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B87" s="6">
         <v>48</v>
@@ -1556,7 +1553,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B88" s="6">
         <v>49</v>
@@ -1567,7 +1564,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" s="6">
         <v>51</v>
@@ -1578,7 +1575,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B90" s="6">
         <v>53</v>
@@ -1589,7 +1586,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B91" s="6" t="e">
         <v>#N/A</v>
@@ -1600,7 +1597,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B92" s="6">
         <v>55</v>
@@ -1611,7 +1608,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B93" s="6">
         <v>8</v>
@@ -1622,7 +1619,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B94" s="6">
         <v>9</v>
@@ -1633,7 +1630,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B95" s="6">
         <v>12</v>
@@ -1644,7 +1641,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B96" s="6">
         <v>13</v>
@@ -1655,7 +1652,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B97" s="6">
         <v>15</v>
@@ -1666,7 +1663,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B98" s="6">
         <v>16</v>
@@ -1677,7 +1674,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B99" s="6">
         <v>18</v>
@@ -1688,7 +1685,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B100" s="6">
         <v>17</v>
@@ -1699,7 +1696,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B101" s="6">
         <v>19</v>
@@ -1710,7 +1707,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B102" s="6">
         <v>20</v>
@@ -1721,7 +1718,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B103" s="6">
         <v>21</v>
@@ -1732,7 +1729,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B104" s="6">
         <v>22</v>
@@ -1743,7 +1740,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B105" s="6">
         <v>23</v>
@@ -1754,7 +1751,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B106" s="6">
         <v>24</v>
@@ -1765,7 +1762,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B107" s="6">
         <v>25</v>
@@ -1776,7 +1773,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B108" s="6">
         <v>26</v>
@@ -1787,7 +1784,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B109" s="6">
         <v>27</v>
@@ -1798,7 +1795,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B110" s="6">
         <v>28</v>
@@ -1809,7 +1806,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B111" s="6">
         <v>29</v>
@@ -1820,7 +1817,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B112" s="6">
         <v>31</v>
@@ -1831,7 +1828,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B113" s="6">
         <v>32</v>
@@ -1842,7 +1839,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B114" s="6">
         <v>33</v>
@@ -1853,7 +1850,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B115" s="6">
         <v>34</v>
@@ -1864,7 +1861,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B116" s="6">
         <v>35</v>
@@ -1875,7 +1872,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B117" s="6">
         <v>36</v>
@@ -1886,7 +1883,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B118" s="6">
         <v>37</v>
@@ -1897,7 +1894,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B119" s="6">
         <v>39</v>
@@ -1908,7 +1905,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B120" s="6">
         <v>40</v>
@@ -1919,7 +1916,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B121" s="6">
         <v>41</v>
@@ -1930,7 +1927,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B122" s="6">
         <v>42</v>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B123" s="6">
         <v>44</v>
@@ -1952,7 +1949,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B124" s="6">
         <v>45</v>
@@ -1963,7 +1960,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B125" s="6">
         <v>47</v>
@@ -1974,7 +1971,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B126" s="6">
         <v>48</v>
@@ -1985,7 +1982,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B127" s="6">
         <v>49</v>
@@ -1996,7 +1993,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B128" s="6">
         <v>51</v>
@@ -2007,7 +2004,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B129" s="6">
         <v>53</v>
@@ -2018,7 +2015,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B130" s="6" t="e">
         <v>#N/A</v>
@@ -2029,7 +2026,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B131" s="6">
         <v>55</v>
@@ -2040,7 +2037,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B132" s="6">
         <v>8</v>
@@ -2051,7 +2048,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B133" s="6">
         <v>9</v>
@@ -2062,7 +2059,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B134" s="6">
         <v>12</v>
@@ -2073,7 +2070,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B135" s="6">
         <v>13</v>
@@ -2084,7 +2081,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B136" s="6">
         <v>18</v>
@@ -2095,7 +2092,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B137" s="6">
         <v>17</v>
@@ -2106,7 +2103,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B138" s="6">
         <v>19</v>
@@ -2117,7 +2114,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B139" s="6">
         <v>20</v>
@@ -2128,7 +2125,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B140" s="6">
         <v>21</v>
@@ -2139,7 +2136,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B141" s="6">
         <v>22</v>
@@ -2150,7 +2147,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B142" s="6">
         <v>24</v>
@@ -2161,7 +2158,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B143" s="6">
         <v>25</v>
@@ -2172,7 +2169,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B144" s="6">
         <v>26</v>
@@ -2183,7 +2180,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B145" s="6">
         <v>27</v>
@@ -2194,7 +2191,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B146" s="6">
         <v>28</v>
@@ -2205,7 +2202,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B147" s="6">
         <v>29</v>
@@ -2216,7 +2213,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B148" s="6">
         <v>31</v>
@@ -2227,7 +2224,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B149" s="6">
         <v>32</v>
@@ -2238,7 +2235,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B150" s="6">
         <v>34</v>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B151" s="6">
         <v>35</v>
@@ -2260,7 +2257,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B152" s="6">
         <v>36</v>
@@ -2271,7 +2268,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B153" s="6">
         <v>37</v>
@@ -2282,7 +2279,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B154" s="6">
         <v>39</v>
@@ -2293,7 +2290,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B155" s="6">
         <v>40</v>
@@ -2304,7 +2301,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B156" s="6">
         <v>41</v>
@@ -2315,7 +2312,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B157" s="6">
         <v>42</v>
@@ -2326,7 +2323,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B158" s="6">
         <v>45</v>
@@ -2337,7 +2334,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B159" s="6">
         <v>47</v>
@@ -2348,7 +2345,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B160" s="6">
         <v>48</v>
@@ -2359,7 +2356,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B161" s="6">
         <v>49</v>
@@ -2370,7 +2367,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B162" s="6">
         <v>51</v>
@@ -2381,7 +2378,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B163" s="6">
         <v>53</v>
@@ -2392,7 +2389,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B164" s="6" t="e">
         <v>#N/A</v>
@@ -2403,7 +2400,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B165" s="6">
         <v>55</v>
@@ -2414,7 +2411,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B166" s="6">
         <v>8</v>
@@ -2425,7 +2422,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B167" s="6">
         <v>9</v>
@@ -2436,7 +2433,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B168" s="6">
         <v>12</v>
@@ -2447,7 +2444,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B169" s="6">
         <v>13</v>
@@ -2458,7 +2455,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B170" s="6">
         <v>18</v>
@@ -2469,7 +2466,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B171" s="6">
         <v>17</v>
@@ -2480,7 +2477,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B172" s="6">
         <v>19</v>
@@ -2491,7 +2488,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B173" s="6">
         <v>20</v>
@@ -2502,7 +2499,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B174" s="6">
         <v>21</v>
@@ -2513,7 +2510,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B175" s="6">
         <v>22</v>
@@ -2524,7 +2521,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B176" s="6">
         <v>24</v>
@@ -2535,7 +2532,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B177" s="6">
         <v>25</v>
@@ -2546,7 +2543,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B178" s="6">
         <v>26</v>
@@ -2557,7 +2554,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B179" s="6">
         <v>27</v>
@@ -2568,7 +2565,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B180" s="6">
         <v>28</v>
@@ -2579,7 +2576,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B181" s="6">
         <v>29</v>
@@ -2590,7 +2587,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B182" s="6">
         <v>32</v>
@@ -2601,7 +2598,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B183" s="6">
         <v>34</v>
@@ -2612,7 +2609,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B184" s="6">
         <v>36</v>
@@ -2623,7 +2620,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B185" s="6">
         <v>37</v>
@@ -2634,7 +2631,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B186" s="6">
         <v>39</v>
@@ -2645,7 +2642,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B187" s="6">
         <v>40</v>
@@ -2656,7 +2653,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B188" s="6">
         <v>41</v>
@@ -2667,7 +2664,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B189" s="6">
         <v>42</v>
@@ -2678,7 +2675,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B190" s="6">
         <v>45</v>
@@ -2689,7 +2686,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B191" s="6">
         <v>47</v>
@@ -2700,7 +2697,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B192" s="6">
         <v>48</v>
@@ -2711,7 +2708,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B193" s="6">
         <v>49</v>
@@ -2722,7 +2719,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B194" s="6">
         <v>51</v>
@@ -2733,7 +2730,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B195" s="6">
         <v>53</v>
@@ -2744,7 +2741,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B196" s="6">
         <v>55</v>
@@ -2755,7 +2752,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B197" s="6">
         <v>8</v>
@@ -2766,7 +2763,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B198" s="6">
         <v>9</v>
@@ -2777,7 +2774,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B199" s="6">
         <v>12</v>
@@ -2788,7 +2785,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B200" s="6">
         <v>13</v>
@@ -2799,7 +2796,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B201" s="6">
         <v>18</v>
@@ -2810,7 +2807,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B202" s="6">
         <v>17</v>
@@ -2821,7 +2818,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B203" s="6">
         <v>21</v>
@@ -2832,7 +2829,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B204" s="6">
         <v>22</v>
@@ -2843,7 +2840,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B205" s="6">
         <v>24</v>
@@ -2854,7 +2851,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B206" s="6">
         <v>25</v>
@@ -2865,7 +2862,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B207" s="6">
         <v>26</v>
@@ -2876,7 +2873,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B208" s="6">
         <v>27</v>
@@ -2887,7 +2884,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B209" s="6">
         <v>29</v>
@@ -2898,7 +2895,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B210" s="6">
         <v>34</v>
@@ -2909,7 +2906,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B211" s="6">
         <v>36</v>
@@ -2920,7 +2917,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B212" s="6">
         <v>37</v>
@@ -2931,7 +2928,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B213" s="6">
         <v>39</v>
@@ -2942,7 +2939,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B214" s="6">
         <v>40</v>
@@ -2953,7 +2950,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B215" s="6">
         <v>41</v>
@@ -2964,7 +2961,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B216" s="6">
         <v>42</v>
@@ -2975,7 +2972,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B217" s="6">
         <v>45</v>
@@ -2986,7 +2983,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B218" s="6">
         <v>47</v>
@@ -2997,7 +2994,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B219" s="6">
         <v>48</v>
@@ -3008,7 +3005,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B220" s="6">
         <v>51</v>
@@ -3019,7 +3016,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B221" s="6">
         <v>53</v>
@@ -3030,7 +3027,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B222" s="6">
         <v>55</v>
@@ -3041,7 +3038,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B223" s="6">
         <v>6</v>
@@ -3052,7 +3049,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B224" s="6">
         <v>8</v>
@@ -3063,7 +3060,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B225" s="6">
         <v>12</v>
@@ -3074,7 +3071,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B226" s="6">
         <v>13</v>
@@ -3085,7 +3082,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B227" s="6">
         <v>18</v>
@@ -3096,7 +3093,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B228" s="6">
         <v>17</v>
@@ -3107,7 +3104,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B229" s="6">
         <v>21</v>
@@ -3118,7 +3115,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B230" s="6">
         <v>22</v>
@@ -3129,7 +3126,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B231" s="6">
         <v>24</v>
@@ -3140,7 +3137,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B232" s="6">
         <v>25</v>
@@ -3151,7 +3148,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B233" s="6">
         <v>26</v>
@@ -3162,7 +3159,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B234" s="6">
         <v>27</v>
@@ -3173,7 +3170,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B235" s="6">
         <v>29</v>
@@ -3184,7 +3181,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B236" s="6">
         <v>34</v>
@@ -3195,7 +3192,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B237" s="6">
         <v>36</v>
@@ -3206,7 +3203,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B238" s="6">
         <v>37</v>
@@ -3217,7 +3214,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B239" s="6">
         <v>39</v>
@@ -3228,7 +3225,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B240" s="6">
         <v>42</v>
@@ -3239,7 +3236,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B241" s="6">
         <v>45</v>
@@ -3250,7 +3247,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B242" s="6">
         <v>47</v>
@@ -3261,7 +3258,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B243" s="6">
         <v>48</v>
@@ -3272,7 +3269,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B244" s="6">
         <v>51</v>
@@ -3283,7 +3280,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B245" s="6">
         <v>53</v>
@@ -3294,7 +3291,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B246" s="6">
         <v>55</v>
@@ -3305,7 +3302,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B247" s="6">
         <v>8</v>
@@ -3316,7 +3313,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B248" s="6">
         <v>12</v>
@@ -3327,7 +3324,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B249" s="6">
         <v>13</v>
@@ -3338,7 +3335,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B250" s="6">
         <v>18</v>
@@ -3349,7 +3346,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B251" s="6">
         <v>17</v>
@@ -3360,7 +3357,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B252" s="6">
         <v>24</v>
@@ -3371,7 +3368,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B253" s="6">
         <v>25</v>
@@ -3382,7 +3379,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B254" s="6">
         <v>26</v>
@@ -3393,7 +3390,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B255" s="6">
         <v>27</v>
@@ -3404,7 +3401,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B256" s="6">
         <v>29</v>
@@ -3415,7 +3412,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B257" s="6">
         <v>34</v>
@@ -3426,7 +3423,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B258" s="6">
         <v>36</v>
@@ -3437,7 +3434,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B259" s="6">
         <v>37</v>
@@ -3448,7 +3445,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B260" s="6">
         <v>39</v>
@@ -3459,7 +3456,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B261" s="6">
         <v>42</v>
@@ -3470,7 +3467,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B262" s="6">
         <v>45</v>
@@ -3481,7 +3478,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B263" s="6">
         <v>47</v>
@@ -3492,7 +3489,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B264" s="6">
         <v>48</v>
@@ -3503,7 +3500,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B265" s="6">
         <v>51</v>
@@ -3514,7 +3511,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B266" s="6">
         <v>53</v>
@@ -3525,7 +3522,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B267" s="6">
         <v>55</v>
@@ -3536,7 +3533,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B268" s="6">
         <v>12</v>
@@ -3547,7 +3544,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B269" s="6">
         <v>13</v>
@@ -3558,7 +3555,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B270" s="6">
         <v>18</v>
@@ -3569,7 +3566,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B271" s="6">
         <v>17</v>
@@ -3580,7 +3577,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B272" s="6">
         <v>24</v>
@@ -3591,7 +3588,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B273" s="6">
         <v>25</v>
@@ -3602,7 +3599,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B274" s="6">
         <v>26</v>
@@ -3613,7 +3610,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B275" s="6">
         <v>27</v>
@@ -3624,7 +3621,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B276" s="6">
         <v>29</v>
@@ -3635,7 +3632,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B277" s="6">
         <v>34</v>
@@ -3646,7 +3643,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B278" s="6">
         <v>36</v>
@@ -3657,7 +3654,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B279" s="6">
         <v>37</v>
@@ -3668,7 +3665,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B280" s="6">
         <v>39</v>
@@ -3679,7 +3676,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B281" s="6">
         <v>42</v>
@@ -3690,7 +3687,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B282" s="6">
         <v>47</v>
@@ -3701,7 +3698,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B283" s="6">
         <v>48</v>
@@ -3712,7 +3709,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B284" s="6">
         <v>51</v>
@@ -3723,7 +3720,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B285" s="6">
         <v>53</v>
@@ -3734,7 +3731,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B286" s="6">
         <v>55</v>
@@ -3745,7 +3742,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B287" s="6">
         <v>12</v>
@@ -3756,7 +3753,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B288" s="6">
         <v>13</v>
@@ -3767,7 +3764,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B289" s="6">
         <v>18</v>
@@ -3778,7 +3775,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B290" s="6">
         <v>17</v>
@@ -3789,7 +3786,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B291" s="6">
         <v>25</v>
@@ -3800,7 +3797,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B292" s="6">
         <v>26</v>
@@ -3811,7 +3808,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B293" s="6">
         <v>34</v>
@@ -3822,7 +3819,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B294" s="6">
         <v>36</v>
@@ -3833,7 +3830,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B295" s="6">
         <v>37</v>
@@ -3844,7 +3841,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B296" s="6">
         <v>39</v>
@@ -3855,7 +3852,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B297" s="6">
         <v>42</v>
@@ -3866,7 +3863,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B298" s="6">
         <v>47</v>
@@ -3877,7 +3874,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B299" s="6">
         <v>48</v>
@@ -3888,7 +3885,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B300" s="6">
         <v>51</v>
@@ -3899,7 +3896,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B301" s="6">
         <v>53</v>
@@ -3910,7 +3907,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B302" s="6">
         <v>12</v>
@@ -3921,7 +3918,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B303" s="6">
         <v>13</v>
@@ -3932,7 +3929,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B304" s="6">
         <v>17</v>
@@ -3943,7 +3940,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B305" s="6">
         <v>26</v>
@@ -3954,7 +3951,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B306" s="6">
         <v>34</v>
@@ -3965,7 +3962,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B307" s="6">
         <v>36</v>
@@ -3976,7 +3973,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B308" s="6">
         <v>37</v>
@@ -3987,7 +3984,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B309" s="6">
         <v>39</v>
@@ -3998,7 +3995,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B310" s="6">
         <v>42</v>
@@ -4009,7 +4006,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B311" s="6">
         <v>48</v>
@@ -4020,7 +4017,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B312" s="6">
         <v>51</v>
@@ -4031,7 +4028,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B313" s="6">
         <v>53</v>
@@ -4042,7 +4039,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B314" s="6">
         <v>12</v>
@@ -4053,7 +4050,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B315" s="6">
         <v>13</v>
@@ -4064,7 +4061,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B316" s="6">
         <v>17</v>
@@ -4075,7 +4072,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B317" s="6">
         <v>26</v>
@@ -4086,7 +4083,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B318" s="6">
         <v>34</v>
@@ -4097,7 +4094,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B319" s="6">
         <v>36</v>
@@ -4108,7 +4105,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B320" s="6">
         <v>37</v>
@@ -4119,7 +4116,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B321" s="6">
         <v>39</v>
@@ -4130,7 +4127,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B322" s="6">
         <v>42</v>
@@ -4141,7 +4138,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B323" s="6">
         <v>48</v>
@@ -4152,7 +4149,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B324" s="6">
         <v>51</v>
@@ -4163,7 +4160,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B325" s="6">
         <v>6</v>
@@ -4174,7 +4171,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B326" s="6">
         <v>12</v>
@@ -4185,7 +4182,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B327" s="6">
         <v>13</v>
@@ -4196,7 +4193,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B328" s="6">
         <v>17</v>
@@ -4207,7 +4204,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B329" s="6">
         <v>26</v>
@@ -4218,7 +4215,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B330" s="6">
         <v>34</v>
@@ -4229,7 +4226,7 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B331" s="6">
         <v>36</v>
@@ -4240,7 +4237,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B332" s="6">
         <v>37</v>
@@ -4251,7 +4248,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B333" s="6">
         <v>39</v>
@@ -4262,7 +4259,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B334" s="6">
         <v>42</v>
@@ -4273,7 +4270,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B335" s="6">
         <v>48</v>
@@ -4284,7 +4281,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B336" s="6">
         <v>6</v>
@@ -4295,7 +4292,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B337" s="6">
         <v>12</v>
@@ -4306,7 +4303,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B338" s="6">
         <v>13</v>
@@ -4317,7 +4314,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B339" s="6">
         <v>17</v>
@@ -4328,7 +4325,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B340" s="6">
         <v>26</v>
@@ -4339,7 +4336,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B341" s="6">
         <v>36</v>
@@ -4350,7 +4347,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B342" s="6">
         <v>37</v>
@@ -4361,7 +4358,7 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B343" s="6">
         <v>39</v>
@@ -4372,7 +4369,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B344" s="6">
         <v>42</v>
@@ -4383,7 +4380,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B345" s="6">
         <v>48</v>
@@ -4394,7 +4391,7 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B346" s="6">
         <v>6</v>
@@ -4405,7 +4402,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B347" s="6">
         <v>12</v>
@@ -4416,7 +4413,7 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B348" s="6">
         <v>13</v>
@@ -4427,7 +4424,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B349" s="6">
         <v>17</v>
@@ -4438,7 +4435,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B350" s="6">
         <v>26</v>
@@ -4449,7 +4446,7 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B351" s="6">
         <v>36</v>
@@ -4460,7 +4457,7 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B352" s="6">
         <v>39</v>
@@ -4471,7 +4468,7 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B353" s="6">
         <v>42</v>
@@ -4482,7 +4479,7 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B354" s="6">
         <v>48</v>
@@ -4493,7 +4490,7 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B355" s="6">
         <v>12</v>
@@ -4504,7 +4501,7 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B356" s="6">
         <v>17</v>
@@ -4515,7 +4512,7 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B357" s="6">
         <v>36</v>
@@ -4526,7 +4523,7 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B358" s="6">
         <v>39</v>
@@ -4537,7 +4534,7 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B359" s="6">
         <v>42</v>
@@ -4548,7 +4545,7 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B360" s="6">
         <v>48</v>
@@ -4559,7 +4556,7 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B361" s="6">
         <v>12</v>
@@ -4570,7 +4567,7 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B362" s="6">
         <v>17</v>
@@ -4581,7 +4578,7 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A363" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B363" s="6">
         <v>36</v>
@@ -4592,7 +4589,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A364" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B364" s="6">
         <v>39</v>
@@ -4603,7 +4600,7 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B365" s="6">
         <v>42</v>
@@ -4614,7 +4611,7 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B366" s="6">
         <v>48</v>
@@ -4625,7 +4622,7 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A367" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B367" s="6">
         <v>6</v>
@@ -4636,7 +4633,7 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A368" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B368" s="6">
         <v>12</v>
@@ -4647,7 +4644,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B369" s="6">
         <v>17</v>
@@ -4658,7 +4655,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B370" s="6">
         <v>36</v>
@@ -4669,7 +4666,7 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B371" s="6">
         <v>42</v>
@@ -4680,7 +4677,7 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B372" s="6">
         <v>48</v>
@@ -4691,7 +4688,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B373" s="6">
         <v>12</v>
@@ -4702,7 +4699,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B374" s="6">
         <v>17</v>
@@ -4713,7 +4710,7 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B375" s="6">
         <v>36</v>
@@ -4724,7 +4721,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B376" s="6">
         <v>42</v>
@@ -4735,7 +4732,7 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B377" s="6">
         <v>48</v>
@@ -4746,7 +4743,7 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B378" s="6">
         <v>12</v>
@@ -4757,7 +4754,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B379" s="6">
         <v>36</v>
@@ -4768,7 +4765,7 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B380" s="6">
         <v>48</v>
@@ -4779,7 +4776,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B381" s="6">
         <v>12</v>
@@ -4790,7 +4787,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B382" s="6">
         <v>36</v>
@@ -4801,7 +4798,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B383" s="6">
         <v>48</v>
@@ -4812,7 +4809,7 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B384" s="6">
         <v>12</v>
@@ -4823,7 +4820,7 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B385" s="6">
         <v>36</v>
@@ -4834,7 +4831,7 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B386" s="6">
         <v>48</v>
@@ -4845,7 +4842,7 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A387" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B387" s="6">
         <v>12</v>
@@ -4856,7 +4853,7 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A388" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B388" s="6">
         <v>36</v>
@@ -4867,7 +4864,7 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A389" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B389" s="6">
         <v>48</v>
@@ -4878,7 +4875,7 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A390" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B390" s="6">
         <v>12</v>
@@ -4889,7 +4886,7 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A391" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B391" s="6">
         <v>36</v>
@@ -4900,7 +4897,7 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A392" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B392" s="6">
         <v>48</v>
@@ -4911,7 +4908,7 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A393" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B393" s="6">
         <v>12</v>
@@ -4922,7 +4919,7 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A394" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B394" s="6">
         <v>36</v>
@@ -4933,7 +4930,7 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A395" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B395" s="6">
         <v>48</v>
@@ -4944,7 +4941,7 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A396" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B396" s="6">
         <v>12</v>
@@ -4955,7 +4952,7 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B397" s="6">
         <v>36</v>
@@ -4966,7 +4963,7 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B398" s="6">
         <v>48</v>
@@ -4977,7 +4974,7 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B399" s="6">
         <v>12</v>
@@ -4988,7 +4985,7 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B400" s="6">
         <v>36</v>
@@ -4999,7 +4996,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B401" s="6">
         <v>48</v>
@@ -5010,7 +5007,7 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B402" s="6">
         <v>12</v>
@@ -5021,7 +5018,7 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B403" s="6">
         <v>36</v>
@@ -5032,7 +5029,7 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B404" s="6">
         <v>48</v>
@@ -5043,7 +5040,7 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B405" s="6">
         <v>6</v>
@@ -5054,7 +5051,7 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B406" s="6">
         <v>48</v>
@@ -5065,7 +5062,7 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B407" s="6">
         <v>6</v>
@@ -5076,7 +5073,7 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B408" s="6">
         <v>48</v>
@@ -5087,7 +5084,7 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B409" s="6">
         <v>6</v>
@@ -5098,7 +5095,7 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B410" s="6">
         <v>48</v>
@@ -5109,7 +5106,7 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B411" s="6">
         <v>6</v>
@@ -5120,7 +5117,7 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B412" s="6">
         <v>48</v>
@@ -5131,7 +5128,7 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B413" s="6">
         <v>6</v>
@@ -5142,7 +5139,7 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B414" s="6">
         <v>48</v>
@@ -5153,7 +5150,7 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B415" s="6">
         <v>48</v>
@@ -5164,7 +5161,7 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B416" s="6">
         <v>6</v>
@@ -5175,7 +5172,7 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B417" s="6">
         <v>48</v>
@@ -5186,7 +5183,7 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B418" s="6">
         <v>6</v>
@@ -5197,7 +5194,7 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B419" s="6">
         <v>48</v>
@@ -5208,7 +5205,7 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B420" s="6">
         <v>48</v>
@@ -5219,7 +5216,7 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B421" s="6">
         <v>6</v>
@@ -5230,7 +5227,7 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B422" s="6">
         <v>6</v>
@@ -5241,7 +5238,7 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B423" s="6">
         <v>6</v>
@@ -5252,7 +5249,7 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B424" s="6">
         <v>6</v>
@@ -5263,7 +5260,7 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B425" s="6">
         <v>6</v>
@@ -5274,7 +5271,7 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B426" s="6">
         <v>6</v>
@@ -5285,7 +5282,7 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B427" s="6">
         <v>6</v>
@@ -5296,7 +5293,7 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B428" s="6">
         <v>6</v>
@@ -5307,7 +5304,7 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B429" s="6">
         <v>6</v>
@@ -5318,7 +5315,7 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B430" s="6">
         <v>6</v>
@@ -5329,79 +5326,79 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B431" s="6">
         <v>10</v>
       </c>
-      <c r="C431" s="7" t="s">
-        <v>5</v>
+      <c r="C431" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B432" s="6">
         <v>11</v>
       </c>
-      <c r="C432" s="7" t="s">
-        <v>5</v>
+      <c r="C432" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A433" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B433" s="6">
         <v>30</v>
       </c>
-      <c r="C433" s="7" t="s">
-        <v>5</v>
+      <c r="C433" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B434" s="6">
         <v>38</v>
       </c>
-      <c r="C434" s="7" t="s">
-        <v>5</v>
+      <c r="C434" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B435" s="6">
         <v>46</v>
       </c>
-      <c r="C435" s="7" t="s">
-        <v>5</v>
+      <c r="C435" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B436" s="6">
         <v>50</v>
       </c>
-      <c r="C436" s="7" t="s">
-        <v>5</v>
+      <c r="C436" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B437" s="6">
         <v>56</v>
       </c>
-      <c r="C437" s="7" t="s">
-        <v>5</v>
+      <c r="C437" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>